<commit_message>
updated BOM resistor values
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://quantumhti.sharepoint.com/sites/company/Shared Documents/Quantum Integration/Engineering/Quantum Hardware/DIY Kits/Q-PCB-003/Four Motors Rev F/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="13_ncr:1_{49EE4D52-1356-114E-BC89-81BF49034CCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{34E20056-29A2-934D-A7BB-C2FB71A8AE46}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="13_ncr:1_{49EE4D52-1356-114E-BC89-81BF49034CCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AAFB6247-9B80-254C-BE18-5831299E31C1}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340" xr2:uid="{E11B78B7-CBD0-0547-AFF9-37277F972DF5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{E11B78B7-CBD0-0547-AFF9-37277F972DF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -156,9 +156,6 @@
     <t>https://www.amazon.com/SIQUK-Resistors-Resistor-Assortment-Experiments/dp/B07PTNN78Z/ref=sr_1_1_sspa?dchild=1&amp;keywords=elegoo+resistor+kit&amp;qid=1598677049&amp;sr=8-1-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyM0o5MTU1RjE0QlRMJmVuY3J5cHRlZElkPUEwODc3MjQ5M1JXSUhLNkZVQkJLVyZlbmNyeXB0ZWRBZElkPUExMDA5OTIzM0NRWjNFOFFaUFBLViZ3aWRnZXROYW1lPXNwX2F0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=</t>
   </si>
   <si>
-    <t>3.8k</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -205,6 +202,9 @@
   </si>
   <si>
     <t>28 pin carrier</t>
+  </si>
+  <si>
+    <t>3.9k</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -791,13 +791,13 @@
         <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>37</v>
@@ -814,22 +814,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="I10" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -837,22 +837,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1">
         <v>5</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" s="1">
         <v>0.1</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -860,19 +860,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="I12" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -880,19 +880,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="I13" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -900,7 +900,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" s="1">
         <v>2</v>
@@ -912,7 +912,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -938,21 +938,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D595B56E1980314DA4E383B61D36AA9D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a773466fb6781862f5fffa930edfaf6b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="97031774-c0c7-48a9-a8e1-3722ddd0f879" xmlns:ns3="a32bd177-85eb-4316-9671-26122bedec74" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6f56f6a42c70e0389f7759d2936d7139" ns2:_="" ns3:_="">
     <xsd:import namespace="97031774-c0c7-48a9-a8e1-3722ddd0f879"/>
@@ -1169,32 +1154,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F46DBAAA-4D3A-4026-9049-CAAAC23F78E1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="97031774-c0c7-48a9-a8e1-3722ddd0f879"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="a32bd177-85eb-4316-9671-26122bedec74"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ED18E5C-7CF9-4494-98F8-0E2F5EED4C77}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27BDAEA5-FCBE-4237-95B9-98FC207DC0AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1211,4 +1186,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ED18E5C-7CF9-4494-98F8-0E2F5EED4C77}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F46DBAAA-4D3A-4026-9049-CAAAC23F78E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a32bd177-85eb-4316-9671-26122bedec74"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="97031774-c0c7-48a9-a8e1-3722ddd0f879"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>